<commit_message>
Atualizações de pastas e arquivos
</commit_message>
<xml_diff>
--- a/Demais/Loggi_Issue_Tracker.xlsx
+++ b/Demais/Loggi_Issue_Tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Perfis SAP" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2072" uniqueCount="1546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2206" uniqueCount="1598">
   <si>
     <t xml:space="preserve">user</t>
   </si>
@@ -4209,13 +4209,10 @@
     <t xml:space="preserve">ID do relator</t>
   </si>
   <si>
-    <t xml:space="preserve">Campo personalizado (Status do pacote)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Descrição</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17081</t>
+    <t xml:space="preserve">JIRAFIN-17897</t>
   </si>
   <si>
     <t xml:space="preserve">Tarefa pendente</t>
@@ -4228,655 +4225,892 @@
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *JULIA.TEIXEIRA@LOGGI.COM*. 
+ Favor revogar acessos de  *JOSE.RODRIGUESPAULA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17080</t>
+    <t xml:space="preserve">JIRAFIN-17895</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *PATRICK.RAMOS@LOGGI.COM*. 
+ Favor revogar acessos de  *GABRIEL.OLIVEIRASILVA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17079</t>
+    <t xml:space="preserve">JIRAFIN-17894</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *CRISTINA.GAINO@LOGGI.COM*. 
+ Favor revogar acessos de  *BRENDA.GABRIELLY@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17076</t>
+    <t xml:space="preserve">JIRAFIN-17893</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *KAUA.SALES@LOGGI.COM*. 
+ Favor revogar acessos de  *jucelio.oliveira@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17075</t>
+    <t xml:space="preserve">JIRAFIN-17892</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *GENEISSON.FERREIRA@LOGGI.COM*. 
+ Favor revogar acessos de  *RODRIGOOLIVEIRA.MELLO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17074</t>
+    <t xml:space="preserve">JIRAFIN-17891</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *marcela.oliveira@loggi.com*. 
+ Favor revogar acessos de  *FELIPE.BRAGA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17073</t>
+    <t xml:space="preserve">JIRAFIN-17890</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ITALO.JOAOSILVA@LOGGI.COM*. 
+ Favor revogar acessos de  *JULIANA.SANTANA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17072</t>
+    <t xml:space="preserve">JIRAFIN-17889</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *LUIZ.JULIO@LOGGI.COM*. 
+ Favor revogar acessos de  *REILANE.FERREIRA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17071</t>
+    <t xml:space="preserve">JIRAFIN-17888</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *MATEUS.ESDRAS@LOGGI.COM*. 
+ Favor revogar acessos de  *DAVID.PENA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17070</t>
+    <t xml:space="preserve">JIRAFIN-17887</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *PEDRO.MIELMICZUK@LOGGI.COM*. 
+ Favor revogar acessos de  *RAMON.BRANDISILVA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17069</t>
+    <t xml:space="preserve">JIRAFIN-17886</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *carlos.dosantos@loggi.com*. 
+ Favor revogar acessos de  *LUCAS.RAMOS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17067</t>
+    <t xml:space="preserve">JIRAFIN-17885</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *VINICIUS.ALVES@LOGGI.COM*. 
+ Favor revogar acessos de  *lennon.azevedo@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17066</t>
+    <t xml:space="preserve">JIRAFIN-17884</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *lucas.almeida@loggi.com*. 
+ Favor revogar acessos de  *wenderson.santos@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17065</t>
+    <t xml:space="preserve">JIRAFIN-17883</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *JOHANE.JEAN@LOGGI.COM*. 
+ Favor revogar acessos de  *JADIENE.CONCEICAO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17064</t>
+    <t xml:space="preserve">JIRAFIN-17882</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ANA.PAULALIMA@LOGGI.COM*. 
+ Favor revogar acessos de  *EDENILSONANZOLIN@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17063</t>
+    <t xml:space="preserve">JIRAFIN-17881</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *MATEUS.TEIXEIRA@LOGGI.COM*. 
+ Favor revogar acessos de  *CARLOS.FERRARI@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17062</t>
+    <t xml:space="preserve">JIRAFIN-17880</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ygor.silva@loggi.com*. 
+ Favor revogar acessos de  *GABRIEL.LUCASSANTANA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17061</t>
+    <t xml:space="preserve">JIRAFIN-17879</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *vivian.alves@loggi.com*. 
+ Favor revogar acessos de  *LYANDRA.DIAS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17059</t>
+    <t xml:space="preserve">JIRAFIN-17878</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *JORGIANY.FERNANDES@LOGGI.COM*. 
+ Favor revogar acessos de  *jean.dias@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17058</t>
+    <t xml:space="preserve">JIRAFIN-17877</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *fabio.rocha@loggi.com*. 
+ Favor revogar acessos de  *INGRID.COELHO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17056</t>
+    <t xml:space="preserve">JIRAFIN-17876</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ILSONEY.VASCONCELOS@LOGGI.COM*. 
+ Favor revogar acessos de  *PAULAFERNANDA.SANTOS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17055</t>
+    <t xml:space="preserve">JIRAFIN-17875</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *VINICIUS.CORREIA@LOGGI.COM*. 
+ Favor revogar acessos de  *ANA.FELIPE@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17053</t>
+    <t xml:space="preserve">JIRAFIN-17874</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *FERNANDO.ROSA@LOGGI.COM*. 
+ Favor revogar acessos de  *THALITA.RIBAS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17052</t>
+    <t xml:space="preserve">JIRAFIN-17873</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *DEIVISON.MIRANDA@LOGGI.COM*. 
+ Favor revogar acessos de  *TAIS.GODOI@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17050</t>
+    <t xml:space="preserve">JIRAFIN-17872</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *VINICIUSRODRIGUES@LOGGI.COM*. 
+ Favor revogar acessos de  *HENRIQUE.LOURO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17047</t>
+    <t xml:space="preserve">JIRAFIN-17871</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *CELIO.OLIVEIRA@LOGGI.COM*. 
+ Favor revogar acessos de  *KATIA.LIMA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17046</t>
+    <t xml:space="preserve">JIRAFIN-17867</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17866</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *RAIZA.BUENO@LOGGI.COM*. 
+ Favor revogar acessos de  *KAREN.FREITAS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17045</t>
+    <t xml:space="preserve">JIRAFIN-17865</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *LUCIANO.OLIVEIRA@LOGGI.COM*. 
+ Favor revogar acessos de  *IVAN.JUNIOR@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17044</t>
+    <t xml:space="preserve">JIRAFIN-17864</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *raissa.bicalho@loggi.com*. 
+ Favor revogar acessos de  *VINICIUS.RAMON@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17043</t>
+    <t xml:space="preserve">JIRAFIN-17863</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *erlane.souza@loggi.com*. 
+ Favor revogar acessos de  *rodrigo.jesus@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17041</t>
+    <t xml:space="preserve">JIRAFIN-17862</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *LUCASFERNANDES.SILVA@LOGGI.COM*. 
+ Favor revogar acessos de  *F.OLIVEIRA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17039</t>
+    <t xml:space="preserve">JIRAFIN-17861</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ANACARVALHO.SOUZA@LOGGI.COM*. 
+ Favor revogar acessos de  *LEONARDO.SANTOSSILVA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17038</t>
+    <t xml:space="preserve">JIRAFIN-17860</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *GUILHERME.MENDONCA@LOGGI.COM*. 
+ Favor revogar acessos de  *VANESSA.ANUNCIACAO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17037</t>
+    <t xml:space="preserve">JIRAFIN-17859</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *OZANA.CARDOSO@LOGGI.COM*. 
+ Favor revogar acessos de  *luydson.santos@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17036</t>
+    <t xml:space="preserve">JIRAFIN-17858</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *EVELIN.CARVALHO@LOGGI.COM*. 
+ Favor revogar acessos de  *RAILAN.DANTAS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17035</t>
+    <t xml:space="preserve">JIRAFIN-17857</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *CLAUDIANE.SILVA@LOGGI.COM*. 
+ Favor revogar acessos de  *jeferson.dias@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17034</t>
+    <t xml:space="preserve">JIRAFIN-17856</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *JOAOPAULO.SOARES@LOGGI.COM*. 
+ Favor revogar acessos de  *F.SILVA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17033</t>
+    <t xml:space="preserve">JIRAFIN-17855</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *LUIZ.SEGALLA@LOGGI.COM*. 
+ Favor revogar acessos de  *DIONES.PESSOA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17032</t>
+    <t xml:space="preserve">JIRAFIN-17854</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *angela.souza@loggi.com*. 
+ Favor revogar acessos de  *ELI.DIAS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17031</t>
+    <t xml:space="preserve">JIRAFIN-17852</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *luciene.rocha@loggi.com*. 
+ Favor revogar acessos de  *vanderson.damasceno@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17027</t>
+    <t xml:space="preserve">JIRAFIN-17851</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *CLERISTON.JESUS@LOGGI.COM*. 
+ Favor revogar acessos de  *WENDELL.SANTOS@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17026</t>
+    <t xml:space="preserve">JIRAFIN-17850</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *maria.eunice@loggi.com*. 
+ Favor revogar acessos de  *ISABELLY.CARMO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17025</t>
+    <t xml:space="preserve">JIRAFIN-17849</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *LEIDIANE.SOUZA@LOGGI.COM*. 
+ Favor revogar acessos de  *GABRIELA.DOMICIANO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17024</t>
+    <t xml:space="preserve">JIRAFIN-17848</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *leonardo.mesquita@loggi.com*. 
+ Favor revogar acessos de  *ALICIA.ANDRADE@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17019</t>
+    <t xml:space="preserve">JIRAFIN-17847</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *MARIA.FERNANDA@LOGGI.COM*. 
+ Favor revogar acessos de  *VICTOR.MOREIRA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17018</t>
+    <t xml:space="preserve">JIRAFIN-17846</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *MIKAELLY.GOMES@LOGGI.COM*. 
+ Favor revogar acessos de  *lucas.andrade@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17017</t>
+    <t xml:space="preserve">JIRAFIN-17845</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *raphael.gil@loggi.com*. 
+ Favor revogar acessos de  *YAGO.OLIVEIRA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17016</t>
+    <t xml:space="preserve">JIRAFIN-17844</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *MANOEL.SILVA@LOGGI.COM*. 
+ Favor revogar acessos de  *rodrigo.pereira@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17014</t>
+    <t xml:space="preserve">JIRAFIN-17843</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ARTUR.MERCES@LOGGI.COM*. 
+ Favor revogar acessos de  *WESLEY.BARBOSA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17013</t>
+    <t xml:space="preserve">JIRAFIN-17842</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *deyvid.valadares@loggi.com*. 
+ Favor revogar acessos de  *KEMILLI.ALVES@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17010</t>
+    <t xml:space="preserve">JIRAFIN-17841</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *JENYFFER.SOUZA@LOGGI.COM*. 
+ Favor revogar acessos de  *GIOVANI.FIGUEREDO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17009</t>
+    <t xml:space="preserve">JIRAFIN-17840</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *PEDRO.AQUINO@LOGGI.COM*. 
+ Favor revogar acessos de  *LETICIA.ASSUNCAO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17008</t>
+    <t xml:space="preserve">JIRAFIN-17839</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *PEDRO.FALCAO@LOGGI.COM*. 
+ Favor revogar acessos de  *GUSTAVO.CAVALCANTE@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17007</t>
+    <t xml:space="preserve">JIRAFIN-17838</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *LAURA.SANTOS@LOGGI.COM*. 
+ Favor revogar acessos de  *PATRICIA.FLORIANO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17006</t>
+    <t xml:space="preserve">JIRAFIN-17837</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *KAUANY.SOARES@LOGGI.COM*. 
+ Favor revogar acessos de  *FABRICIA.BERTELI@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17005</t>
+    <t xml:space="preserve">JIRAFIN-17836</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *JAMILLY.GONCALVES@LOGGI.COM*. 
+ Favor revogar acessos de  *YOHANNA.CAVALCANTI@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17004</t>
+    <t xml:space="preserve">JIRAFIN-17835</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *GUSTAVOHENRIQUE.FERREIRA@LOGGI.COM*. 
+ Favor revogar acessos de  *MARIA.FURTADO@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17003</t>
+    <t xml:space="preserve">JIRAFIN-17834</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ERIK.OLIVEIRA@LOGGI.COM*. 
+ Favor revogar acessos de  *THAIS.FAGUNDES@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17002</t>
+    <t xml:space="preserve">JIRAFIN-17833</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *CAMILLY.SOUZA@LOGGI.COM*. 
+ Favor revogar acessos de  *NATHASCHA.GONCALVES@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17001</t>
+    <t xml:space="preserve">JIRAFIN-17832</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *ASHLEY.SILVA@LOGGI.COM*. 
+ Favor revogar acessos de  *ALLYNE.CAPUANI@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-17000</t>
+    <t xml:space="preserve">JIRAFIN-17831</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *HALFREDY.AQUINO@LOGGI.COM*. 
+ Favor revogar acessos de  *RHAISSA.NASSER@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16999</t>
+    <t xml:space="preserve">JIRAFIN-17830</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *HENRIQUE.MOURA@LOGGI.COM*. 
+ Favor revogar acessos de  *DAVI.ERIC@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16998</t>
+    <t xml:space="preserve">JIRAFIN-17829</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *VITORUGO.SOUZA@LOGGI.COM*. 
+ Favor revogar acessos de  *ROSENO.SILVA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16996</t>
+    <t xml:space="preserve">JIRAFIN-17828</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *FERNANDO.BARBOSA@LOGGI.COM*. 
+ Favor revogar acessos de  *edmar.resende@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16995</t>
+    <t xml:space="preserve">JIRAFIN-17827</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *RAFAELLA.GONCALVES@LOGGI.COM*. 
+ Favor revogar acessos de  *filippe.paiva@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16994</t>
+    <t xml:space="preserve">JIRAFIN-17826</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *MILENA.ASSIS@LOGGI.COM*. 
+ Favor revogar acessos de  *jonathan.cardoso@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16993</t>
+    <t xml:space="preserve">JIRAFIN-17825</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *MARIA.TELES@LOGGI.COM*. 
+ Favor revogar acessos de  *paulo.tiroli@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16992</t>
+    <t xml:space="preserve">JIRAFIN-17824</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *GUSTAVO.BENTO@LOGGI.COM*. 
+ Favor revogar acessos de  *giselle.silva@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16991</t>
+    <t xml:space="preserve">JIRAFIN-17823</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *GUSTAVO.BARBOSA@LOGGI.COM*. 
+ Favor revogar acessos de  *jacqueline.pedreti@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16990</t>
+    <t xml:space="preserve">JIRAFIN-17822</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *YASMIN.NUNES@LOGGI.COM*. 
+ Favor revogar acessos de  *leticia.souza@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16989</t>
+    <t xml:space="preserve">JIRAFIN-17821</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *CAROLINE.MACHADO@LOGGI.COM*. 
+ Favor revogar acessos de  *Leticia.Santolim@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16986</t>
+    <t xml:space="preserve">JIRAFIN-17820</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *HUGO.CORREIA@LOGGI.COM*. 
+ Favor revogar acessos de  *marlon.lisboa@loggi.com*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
   <si>
-    <t xml:space="preserve">JIRAFIN-16985</t>
+    <t xml:space="preserve">JIRAFIN-17819</t>
   </si>
   <si>
     <t xml:space="preserve">Olá pessoal, tudo bem? 
- Favor revogar acessos de  *JACQUELINE.RUANO@LOGGI.COM*. 
+ Favor revogar acessos de  *marcelo.tourinho@loggi.com*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *HENRIQUE.BISPO@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *MARIANA.ASSIS@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17816</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *rogerio.macedo@loggi.com*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17815</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *FLAVIO.EVANGELISTA@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17794</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *JENNIFER.NUNES@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17792</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *camila.santos@loggi.com*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *ELISABETE.FRANCA@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17788</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *MYLELLY.SANTOS@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *SARA.SETUBAL@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *WILLIANE.SANTOS@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17785</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *NAIARA.ANDRADE@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17784</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *CARLA.MELO@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17783</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *ALEXANDRE.LIMA@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17782</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *JENIPHER.STEPHANIE@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17781</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *jonas.junior@loggi.com*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17780</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *MARIA.REJANE@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17779</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *KETYLIN.RODRIGUES@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17778</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *EDUARDO.CANDIDO@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17773</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *MARCOS.ARAGAO@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17772</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *RAFAELA.CARVALHO@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17771</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *thibaud@loggi.com*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *MONIKE.SALES@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *ADRIANO.MENEZES@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17760</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *alexander.santos@loggi.com*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17758</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *JONATHAN.TEIXEIRA@LOGGI.COM*. 
+ Esta é uma mensagem automática. 
+ Obrigado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JIRAFIN-17756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olá pessoal, tudo bem? 
+ Favor revogar acessos de  *RAPHAEL.COSTA@LOGGI.COM*. 
  Esta é uma mensagem automática. 
  Obrigado</t>
   </si>
@@ -5091,11 +5325,11 @@
   </sheetPr>
   <dimension ref="A1:C501"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A1:A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="2.54"/>
@@ -10587,10 +10821,10 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="1" sqref="A1:A74 F19"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.97"/>
@@ -13344,8 +13578,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -13355,13 +13589,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:A74"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.92"/>
@@ -13391,1468 +13625,2078 @@
       <c r="F1" s="1" t="s">
         <v>1395</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>1396</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>5921786</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1397</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>5838465</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>1400</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>1401</v>
-      </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>5921125</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>1402</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>5838458</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>1403</v>
-      </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>5920883</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>1404</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>5838449</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>1405</v>
-      </c>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>5920876</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>1406</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>5838414</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>1407</v>
-      </c>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>5920870</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>1408</v>
       </c>
-      <c r="B6" s="1" t="n">
-        <v>5838352</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>1409</v>
-      </c>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>5920860</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>1410</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>5838333</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>1411</v>
-      </c>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>1411</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>5920852</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>1412</v>
       </c>
-      <c r="B8" s="1" t="n">
-        <v>5838329</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>1413</v>
-      </c>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>5920769</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>1414</v>
       </c>
-      <c r="B9" s="1" t="n">
-        <v>5838042</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>1415</v>
-      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>5920768</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>1416</v>
       </c>
-      <c r="B10" s="1" t="n">
-        <v>5838041</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>1417</v>
-      </c>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>5920767</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>1418</v>
       </c>
-      <c r="B11" s="1" t="n">
-        <v>5838040</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>1419</v>
-      </c>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>5920750</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>1420</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>5838039</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>1421</v>
-      </c>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>5920749</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>1422</v>
       </c>
-      <c r="B13" s="1" t="n">
-        <v>5837516</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>1423</v>
-      </c>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>5920747</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>1424</v>
       </c>
-      <c r="B14" s="1" t="n">
-        <v>5836803</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>1425</v>
-      </c>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>5919666</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>1426</v>
       </c>
-      <c r="B15" s="1" t="n">
-        <v>5836794</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>1427</v>
-      </c>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>5919462</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>1428</v>
       </c>
-      <c r="B16" s="1" t="n">
-        <v>5836770</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>1429</v>
-      </c>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>5919271</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>1430</v>
       </c>
-      <c r="B17" s="1" t="n">
-        <v>5836504</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>1431</v>
-      </c>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>5919252</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>1432</v>
       </c>
-      <c r="B18" s="1" t="n">
-        <v>5836503</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>1433</v>
-      </c>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>5919245</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>1434</v>
       </c>
-      <c r="B19" s="1" t="n">
-        <v>5836502</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>1435</v>
-      </c>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>5919239</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>1436</v>
       </c>
-      <c r="B20" s="1" t="n">
-        <v>5833652</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>1437</v>
-      </c>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>5919231</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>1438</v>
       </c>
-      <c r="B21" s="1" t="n">
-        <v>5833645</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>1439</v>
-      </c>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>5919227</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>1440</v>
       </c>
-      <c r="B22" s="1" t="n">
-        <v>5832899</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>1441</v>
-      </c>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>5919217</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>1442</v>
       </c>
-      <c r="B23" s="1" t="n">
-        <v>5832746</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>1443</v>
-      </c>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>5919209</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>1444</v>
       </c>
-      <c r="B24" s="1" t="n">
-        <v>5832211</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>1445</v>
-      </c>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>5919199</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>1446</v>
       </c>
-      <c r="B25" s="1" t="n">
-        <v>5832155</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>1447</v>
-      </c>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>1447</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>5919192</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>1448</v>
       </c>
-      <c r="B26" s="1" t="n">
-        <v>5831657</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>1449</v>
-      </c>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>5919191</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>1450</v>
       </c>
-      <c r="B27" s="1" t="n">
-        <v>5831477</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>1398</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>1451</v>
-      </c>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>5831399</v>
+        <v>5918894</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>1453</v>
-      </c>
+      <c r="F28" s="2" t="s">
+        <v>1402</v>
+      </c>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>5831200</v>
+        <v>5918893</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>1455</v>
-      </c>
+      <c r="F29" s="2" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>5831199</v>
+        <v>5918892</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>1457</v>
-      </c>
+      <c r="F30" s="2" t="s">
+        <v>1455</v>
+      </c>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>5831096</v>
+        <v>5918891</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>1459</v>
-      </c>
+      <c r="F31" s="2" t="s">
+        <v>1457</v>
+      </c>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>5830276</v>
+        <v>5918890</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>1461</v>
-      </c>
+      <c r="F32" s="2" t="s">
+        <v>1459</v>
+      </c>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="B33" s="1" t="n">
-        <v>5830199</v>
+        <v>5918299</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>1463</v>
-      </c>
+      <c r="F33" s="2" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="B34" s="1" t="n">
-        <v>5829973</v>
+        <v>5918291</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>1465</v>
-      </c>
+      <c r="F34" s="2" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="B35" s="1" t="n">
-        <v>5829972</v>
+        <v>5918270</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>1467</v>
-      </c>
+      <c r="F35" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="B36" s="1" t="n">
-        <v>5829971</v>
+        <v>5918261</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E36" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>1469</v>
-      </c>
+      <c r="F36" s="2" t="s">
+        <v>1467</v>
+      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="B37" s="1" t="n">
-        <v>5829970</v>
+        <v>5918260</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>1471</v>
-      </c>
+      <c r="F37" s="2" t="s">
+        <v>1469</v>
+      </c>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="B38" s="1" t="n">
-        <v>5829969</v>
+        <v>5918069</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>1473</v>
-      </c>
+      <c r="F38" s="2" t="s">
+        <v>1471</v>
+      </c>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="B39" s="1" t="n">
-        <v>5829968</v>
+        <v>5918063</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>1475</v>
-      </c>
+      <c r="F39" s="2" t="s">
+        <v>1473</v>
+      </c>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
       <c r="B40" s="1" t="n">
-        <v>5829967</v>
+        <v>5918059</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>1477</v>
-      </c>
+      <c r="F40" s="2" t="s">
+        <v>1475</v>
+      </c>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="B41" s="1" t="n">
-        <v>5829952</v>
+        <v>5918052</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>1479</v>
-      </c>
+      <c r="F41" s="2" t="s">
+        <v>1477</v>
+      </c>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="B42" s="1" t="n">
-        <v>5828261</v>
+        <v>5917486</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E42" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>1481</v>
-      </c>
+      <c r="F42" s="2" t="s">
+        <v>1479</v>
+      </c>
+      <c r="G42" s="2"/>
     </row>
     <row r="43" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
       <c r="B43" s="1" t="n">
-        <v>5828249</v>
+        <v>5917198</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>1483</v>
-      </c>
+      <c r="F43" s="2" t="s">
+        <v>1481</v>
+      </c>
+      <c r="G43" s="2"/>
     </row>
     <row r="44" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="B44" s="1" t="n">
-        <v>5828248</v>
+        <v>5917135</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E44" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>1485</v>
-      </c>
+      <c r="F44" s="2" t="s">
+        <v>1483</v>
+      </c>
+      <c r="G44" s="2"/>
     </row>
     <row r="45" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
       <c r="B45" s="1" t="n">
-        <v>5828247</v>
+        <v>5917055</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>1487</v>
-      </c>
+      <c r="F45" s="2" t="s">
+        <v>1485</v>
+      </c>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="B46" s="1" t="n">
-        <v>5826869</v>
+        <v>5917043</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E46" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>1489</v>
-      </c>
+      <c r="F46" s="2" t="s">
+        <v>1487</v>
+      </c>
+      <c r="G46" s="2"/>
     </row>
     <row r="47" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="B47" s="1" t="n">
-        <v>5826838</v>
+        <v>5917025</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E47" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>1491</v>
-      </c>
+      <c r="F47" s="2" t="s">
+        <v>1489</v>
+      </c>
+      <c r="G47" s="2"/>
     </row>
     <row r="48" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="B48" s="1" t="n">
-        <v>5826320</v>
+        <v>5917013</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>1493</v>
-      </c>
+      <c r="F48" s="2" t="s">
+        <v>1491</v>
+      </c>
+      <c r="G48" s="2"/>
     </row>
     <row r="49" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="B49" s="1" t="n">
-        <v>5826319</v>
+        <v>5916994</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="E49" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>1495</v>
-      </c>
+      <c r="F49" s="2" t="s">
+        <v>1493</v>
+      </c>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="B50" s="1" t="n">
-        <v>5825809</v>
+        <v>5916987</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>1497</v>
-      </c>
+      <c r="F50" s="2" t="s">
+        <v>1495</v>
+      </c>
+      <c r="G50" s="2"/>
     </row>
     <row r="51" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="B51" s="1" t="n">
-        <v>5825802</v>
+        <v>5916983</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E51" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>1499</v>
-      </c>
+      <c r="F51" s="2" t="s">
+        <v>1497</v>
+      </c>
+      <c r="G51" s="2"/>
     </row>
     <row r="52" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="B52" s="1" t="n">
-        <v>5825138</v>
+        <v>5916740</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>1501</v>
-      </c>
+      <c r="F52" s="2" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="B53" s="1" t="n">
-        <v>5825137</v>
+        <v>5916739</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E53" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>1503</v>
-      </c>
+      <c r="F53" s="2" t="s">
+        <v>1501</v>
+      </c>
+      <c r="G53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="B54" s="1" t="n">
-        <v>5825136</v>
+        <v>5916738</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E54" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>1505</v>
-      </c>
+      <c r="F54" s="2" t="s">
+        <v>1503</v>
+      </c>
+      <c r="G54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="B55" s="1" t="n">
-        <v>5825135</v>
+        <v>5916737</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>1507</v>
-      </c>
+      <c r="F55" s="2" t="s">
+        <v>1505</v>
+      </c>
+      <c r="G55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="B56" s="1" t="n">
-        <v>5825134</v>
+        <v>5916736</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>1509</v>
-      </c>
+      <c r="F56" s="2" t="s">
+        <v>1507</v>
+      </c>
+      <c r="G56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="B57" s="1" t="n">
-        <v>5825133</v>
+        <v>5916735</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>1511</v>
-      </c>
+      <c r="F57" s="2" t="s">
+        <v>1509</v>
+      </c>
+      <c r="G57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="B58" s="1" t="n">
-        <v>5825132</v>
+        <v>5916676</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>1513</v>
-      </c>
+      <c r="F58" s="2" t="s">
+        <v>1511</v>
+      </c>
+      <c r="G58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="B59" s="1" t="n">
-        <v>5825131</v>
+        <v>5916675</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>1515</v>
-      </c>
+      <c r="F59" s="2" t="s">
+        <v>1513</v>
+      </c>
+      <c r="G59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="B60" s="1" t="n">
-        <v>5825130</v>
+        <v>5916674</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>1517</v>
-      </c>
+      <c r="F60" s="2" t="s">
+        <v>1515</v>
+      </c>
+      <c r="G60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>5825129</v>
+        <v>5916673</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>1519</v>
-      </c>
+      <c r="F61" s="2" t="s">
+        <v>1517</v>
+      </c>
+      <c r="G61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="B62" s="1" t="n">
-        <v>5825093</v>
+        <v>5916672</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>1521</v>
-      </c>
+      <c r="F62" s="2" t="s">
+        <v>1519</v>
+      </c>
+      <c r="G62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="B63" s="1" t="n">
-        <v>5825091</v>
+        <v>5916671</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>1523</v>
-      </c>
+      <c r="F63" s="2" t="s">
+        <v>1521</v>
+      </c>
+      <c r="G63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="B64" s="1" t="n">
-        <v>5825089</v>
+        <v>5916670</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="E64" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>1525</v>
-      </c>
+      <c r="F64" s="2" t="s">
+        <v>1523</v>
+      </c>
+      <c r="G64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="B65" s="1" t="n">
-        <v>5824676</v>
+        <v>5916669</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>1527</v>
-      </c>
+      <c r="F65" s="2" t="s">
+        <v>1525</v>
+      </c>
+      <c r="G65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
       <c r="B66" s="1" t="n">
-        <v>5824290</v>
+        <v>5916668</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="E66" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>1529</v>
-      </c>
+      <c r="F66" s="2" t="s">
+        <v>1527</v>
+      </c>
+      <c r="G66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="B67" s="1" t="n">
-        <v>5824284</v>
+        <v>5916667</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E67" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>1531</v>
-      </c>
+      <c r="F67" s="2" t="s">
+        <v>1529</v>
+      </c>
+      <c r="G67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
       <c r="B68" s="1" t="n">
-        <v>5824279</v>
+        <v>5916666</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="E68" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>1533</v>
-      </c>
+      <c r="F68" s="2" t="s">
+        <v>1531</v>
+      </c>
+      <c r="G68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="B69" s="1" t="n">
-        <v>5824274</v>
+        <v>5916665</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>1535</v>
-      </c>
+      <c r="F69" s="2" t="s">
+        <v>1533</v>
+      </c>
+      <c r="G69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="B70" s="1" t="n">
-        <v>5824268</v>
+        <v>5916664</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="E70" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>1537</v>
-      </c>
+      <c r="F70" s="2" t="s">
+        <v>1535</v>
+      </c>
+      <c r="G70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="B71" s="1" t="n">
-        <v>5824262</v>
+        <v>5916663</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="E71" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>1539</v>
-      </c>
+      <c r="F71" s="2" t="s">
+        <v>1537</v>
+      </c>
+      <c r="G71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="B72" s="1" t="n">
-        <v>5824259</v>
+        <v>5916662</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>1541</v>
-      </c>
+      <c r="F72" s="2" t="s">
+        <v>1539</v>
+      </c>
+      <c r="G72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="B73" s="1" t="n">
-        <v>5823829</v>
+        <v>5916661</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E73" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>1543</v>
-      </c>
+      <c r="F73" s="2" t="s">
+        <v>1541</v>
+      </c>
+      <c r="G73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B74" s="1" t="n">
+        <v>5916660</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>1543</v>
+      </c>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="1" t="s">
         <v>1544</v>
       </c>
-      <c r="B74" s="1" t="n">
-        <v>5823711</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="B75" s="1" t="n">
+        <v>5916659</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>1398</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="E75" s="1" t="s">
         <v>1399</v>
       </c>
-      <c r="E74" s="1" t="s">
-        <v>1400</v>
-      </c>
-      <c r="G74" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>1545</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B76" s="1" t="n">
+        <v>5916658</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="1" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B77" s="1" t="n">
+        <v>5916656</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B78" s="1" t="n">
+        <v>5916616</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B79" s="1" t="n">
+        <v>5915745</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B80" s="1" t="n">
+        <v>5915368</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B81" s="1" t="n">
+        <v>5914973</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="1" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B82" s="1" t="n">
+        <v>5914406</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="1" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B83" s="1" t="n">
+        <v>5914405</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="1" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B84" s="1" t="n">
+        <v>5914404</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="1" t="s">
+        <v>1564</v>
+      </c>
+      <c r="B85" s="1" t="n">
+        <v>5914403</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>1566</v>
+      </c>
+      <c r="B86" s="1" t="n">
+        <v>5914402</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>1568</v>
+      </c>
+      <c r="B87" s="1" t="n">
+        <v>5914401</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>1570</v>
+      </c>
+      <c r="B88" s="1" t="n">
+        <v>5914400</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>1572</v>
+      </c>
+      <c r="B89" s="1" t="n">
+        <v>5914399</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B90" s="1" t="n">
+        <v>5914398</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B91" s="1" t="n">
+        <v>5914177</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>1578</v>
+      </c>
+      <c r="B92" s="1" t="n">
+        <v>5914169</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>1579</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B93" s="1" t="n">
+        <v>5913921</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B94" s="1" t="n">
+        <v>5913092</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>1584</v>
+      </c>
+      <c r="B95" s="1" t="n">
+        <v>5913091</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B96" s="1" t="n">
+        <v>5913041</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>1588</v>
+      </c>
+      <c r="B97" s="1" t="n">
+        <v>5904530</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B98" s="1" t="n">
+        <v>5904523</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B99" s="1" t="n">
+        <v>5904324</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>1594</v>
+      </c>
+      <c r="B100" s="1" t="n">
+        <v>5902797</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B101" s="1" t="n">
+        <v>5902367</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>1397</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>1398</v>
+      </c>
+      <c r="E101" s="1" t="s">
+        <v>1399</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>1597</v>
       </c>
     </row>
   </sheetData>
@@ -14860,8 +15704,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>